<commit_message>
Ad hoc fix to pull_data
pull_data is unable to retrieve annual data at the moment
</commit_message>
<xml_diff>
--- a/data/raw/haver/economic_annual.xlsx
+++ b/data/raw/haver/economic_annual.xlsx
@@ -15,9 +15,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -55,12 +52,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,9 +356,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
@@ -392,8 +385,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
-        <v>25933</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1970-12-31</t>
+        </is>
       </c>
       <c r="D2">
         <v>1088</v>
@@ -403,8 +398,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
-        <v>26298</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1971-12-31</t>
+        </is>
       </c>
       <c r="D3">
         <v>1177.4</v>
@@ -414,8 +411,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
-        <v>26664</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1972-12-31</t>
+        </is>
       </c>
       <c r="D4">
         <v>1265.7</v>
@@ -425,8 +424,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
-        <v>27029</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1973-12-31</t>
+        </is>
       </c>
       <c r="D5">
         <v>1378.8</v>
@@ -436,8 +437,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
-        <v>27394</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1974-12-31</t>
+        </is>
       </c>
       <c r="D6">
         <v>1556</v>
@@ -447,8 +450,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2">
-        <v>27759</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1975-12-31</t>
+        </is>
       </c>
       <c r="C7">
         <v>25.68916666666667</v>
@@ -461,8 +466,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2">
-        <v>28125</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1976-12-31</t>
+        </is>
       </c>
       <c r="C8">
         <v>27.615</v>
@@ -475,8 +482,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2">
-        <v>28490</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1977-12-31</t>
+        </is>
       </c>
       <c r="C9">
         <v>30.92</v>
@@ -489,8 +498,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
-        <v>28855</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1978-12-31</t>
+        </is>
       </c>
       <c r="C10">
         <v>35.61166666666667</v>
@@ -503,8 +514,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
-        <v>29220</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1979-12-31</t>
+        </is>
       </c>
       <c r="C11">
         <v>41.09416666666667</v>
@@ -517,8 +530,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2">
-        <v>29586</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1980-12-31</t>
+        </is>
       </c>
       <c r="C12">
         <v>45.0925</v>
@@ -531,8 +546,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2">
-        <v>29951</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1981-12-31</t>
+        </is>
       </c>
       <c r="C13">
         <v>47.96</v>
@@ -545,8 +562,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2">
-        <v>30316</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1982-12-31</t>
+        </is>
       </c>
       <c r="C14">
         <v>48.94166666666666</v>
@@ -559,8 +578,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2">
-        <v>30681</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1983-12-31</t>
+        </is>
       </c>
       <c r="C15">
         <v>50.45916666666667</v>
@@ -573,8 +594,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2">
-        <v>31047</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1984-12-31</t>
+        </is>
       </c>
       <c r="C16">
         <v>52.84</v>
@@ -587,8 +610,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2">
-        <v>31412</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1985-12-31</t>
+        </is>
       </c>
       <c r="C17">
         <v>55.88500000000001</v>
@@ -601,8 +626,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2">
-        <v>31777</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1986-12-31</t>
+        </is>
       </c>
       <c r="C18">
         <v>60.82166666666666</v>
@@ -615,8 +642,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
-        <v>32142</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1987-12-31</t>
+        </is>
       </c>
       <c r="C19">
         <v>66.26833333333333</v>
@@ -629,8 +658,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2">
-        <v>32508</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>1988-12-31</t>
+        </is>
       </c>
       <c r="C20">
         <v>71.14416666666666</v>
@@ -643,8 +674,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2">
-        <v>32873</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>1989-12-31</t>
+        </is>
       </c>
       <c r="C21">
         <v>75.50833333333334</v>
@@ -657,8 +690,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2">
-        <v>33238</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>1990-12-31</t>
+        </is>
       </c>
       <c r="C22">
         <v>76.935</v>
@@ -671,8 +706,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2">
-        <v>33603</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>1991-12-31</t>
+        </is>
       </c>
       <c r="B23">
         <v>100.3075</v>
@@ -688,8 +725,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2">
-        <v>33969</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>1992-12-31</t>
+        </is>
       </c>
       <c r="B24">
         <v>102.8225</v>
@@ -705,8 +744,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2">
-        <v>34334</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1993-12-31</t>
+        </is>
       </c>
       <c r="B25">
         <v>105.305</v>
@@ -722,8 +763,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2">
-        <v>34699</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>1994-12-31</t>
+        </is>
       </c>
       <c r="B26">
         <v>108.82</v>
@@ -739,8 +782,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2">
-        <v>35064</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>1995-12-31</t>
+        </is>
       </c>
       <c r="B27">
         <v>111.66</v>
@@ -756,8 +801,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2">
-        <v>35430</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>1996-12-31</t>
+        </is>
       </c>
       <c r="B28">
         <v>114.94</v>
@@ -773,8 +820,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2">
-        <v>35795</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>1997-12-31</t>
+        </is>
       </c>
       <c r="B29">
         <v>118.2175</v>
@@ -790,8 +839,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2">
-        <v>36160</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1998-12-31</t>
+        </is>
       </c>
       <c r="B30">
         <v>123.935</v>
@@ -807,8 +858,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2">
-        <v>36525</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>1999-12-31</t>
+        </is>
       </c>
       <c r="B31">
         <v>131.4875</v>
@@ -824,8 +877,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2">
-        <v>36891</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2000-12-31</t>
+        </is>
       </c>
       <c r="B32">
         <v>140.3075</v>
@@ -841,8 +896,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2">
-        <v>37256</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2001-12-31</t>
+        </is>
       </c>
       <c r="B33">
         <v>150.0075</v>
@@ -858,8 +915,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2">
-        <v>37621</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2002-12-31</t>
+        </is>
       </c>
       <c r="B34">
         <v>160.5775</v>
@@ -875,8 +934,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2">
-        <v>37986</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2003-12-31</t>
+        </is>
       </c>
       <c r="B35">
         <v>172.8875</v>
@@ -892,8 +953,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2">
-        <v>38352</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2004-12-31</t>
+        </is>
       </c>
       <c r="B36">
         <v>189.2175</v>
@@ -909,8 +972,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2">
-        <v>38717</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2005-12-31</t>
+        </is>
       </c>
       <c r="B37">
         <v>209.0325</v>
@@ -926,8 +991,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2">
-        <v>39082</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2006-12-31</t>
+        </is>
       </c>
       <c r="B38">
         <v>221.2775</v>
@@ -943,8 +1010,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2">
-        <v>39447</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2007-12-31</t>
+        </is>
       </c>
       <c r="B39">
         <v>221.255</v>
@@ -960,8 +1029,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2">
-        <v>39813</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2008-12-31</t>
+        </is>
       </c>
       <c r="B40">
         <v>203.2025</v>
@@ -977,8 +1048,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2">
-        <v>40178</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2009-12-31</t>
+        </is>
       </c>
       <c r="B41">
         <v>191.0975</v>
@@ -994,8 +1067,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2">
-        <v>40543</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2010-12-31</t>
+        </is>
       </c>
       <c r="B42">
         <v>185.3925</v>
@@ -1011,8 +1086,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2">
-        <v>40908</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2011-12-31</t>
+        </is>
       </c>
       <c r="B43">
         <v>177.56</v>
@@ -1028,8 +1105,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2">
-        <v>41274</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2012-12-31</t>
+        </is>
       </c>
       <c r="B44">
         <v>182.57</v>
@@ -1045,8 +1124,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2">
-        <v>41639</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2013-12-31</t>
+        </is>
       </c>
       <c r="B45">
         <v>195.37</v>
@@ -1062,8 +1143,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2">
-        <v>42004</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2014-12-31</t>
+        </is>
       </c>
       <c r="B46">
         <v>205.12</v>
@@ -1079,8 +1162,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2">
-        <v>42369</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2015-12-31</t>
+        </is>
       </c>
       <c r="B47">
         <v>215.915</v>
@@ -1096,8 +1181,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2">
-        <v>42735</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2016-12-31</t>
+        </is>
       </c>
       <c r="B48">
         <v>228.37</v>
@@ -1113,8 +1200,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2">
-        <v>43100</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2017-12-31</t>
+        </is>
       </c>
       <c r="B49">
         <v>242.775</v>
@@ -1130,8 +1219,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2">
-        <v>43465</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2018-12-31</t>
+        </is>
       </c>
       <c r="B50">
         <v>258.37</v>
@@ -1147,8 +1238,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2">
-        <v>43830</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2019-12-31</t>
+        </is>
       </c>
       <c r="B51">
         <v>271.9300000000001</v>
@@ -1164,14 +1257,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2">
-        <v>44196</v>
-      </c>
-      <c r="B52">
-        <v>257.6916666666667</v>
-      </c>
-      <c r="C52">
-        <v>201.2072222222222</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2020-12-31</t>
+        </is>
       </c>
       <c r="D52">
         <v>21763.5</v>
@@ -1181,14 +1270,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2">
-        <v>44561</v>
-      </c>
-      <c r="B53">
-        <v>262.6638888888889</v>
-      </c>
-      <c r="C53">
-        <v>204.4562962962963</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2021-12-31</t>
+        </is>
       </c>
       <c r="D53">
         <v>22257.4</v>
@@ -1198,14 +1283,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2">
-        <v>44926</v>
-      </c>
-      <c r="B54">
-        <v>264.0951851851852</v>
-      </c>
-      <c r="C54">
-        <v>205.0889506172839</v>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2022-12-31</t>
+        </is>
       </c>
       <c r="D54">
         <v>23013.9</v>
@@ -1215,14 +1296,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2">
-        <v>45291</v>
-      </c>
-      <c r="B55">
-        <v>261.4835802469136</v>
-      </c>
-      <c r="C55">
-        <v>203.5841563786008</v>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2023-12-31</t>
+        </is>
       </c>
       <c r="D55">
         <v>23874.9</v>
@@ -1232,14 +1309,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2">
-        <v>45657</v>
-      </c>
-      <c r="B56">
-        <v>262.7475514403292</v>
-      </c>
-      <c r="C56">
-        <v>204.3764677640603</v>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-12-31</t>
+        </is>
       </c>
       <c r="D56">
         <v>24806.6</v>
@@ -1249,14 +1322,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2">
-        <v>46022</v>
-      </c>
-      <c r="B57">
-        <v>262.775438957476</v>
-      </c>
-      <c r="C57">
-        <v>204.349858253315</v>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
       </c>
       <c r="D57">
         <v>25781</v>
@@ -1266,14 +1335,10 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2">
-        <v>46387</v>
-      </c>
-      <c r="B58">
-        <v>262.3355235482396</v>
-      </c>
-      <c r="C58">
-        <v>204.1034941319921</v>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-12-31</t>
+        </is>
       </c>
       <c r="D58">
         <v>26784.5</v>
@@ -1283,14 +1348,10 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2">
-        <v>46752</v>
-      </c>
-      <c r="B59">
-        <v>262.6195046486816</v>
-      </c>
-      <c r="C59">
-        <v>204.2766067164558</v>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2027-12-31</t>
+        </is>
       </c>
       <c r="D59">
         <v>27817.3</v>
@@ -1300,14 +1361,10 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2">
-        <v>47118</v>
-      </c>
-      <c r="B60">
-        <v>262.5768223847991</v>
-      </c>
-      <c r="C60">
-        <v>204.2433197005876</v>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2028-12-31</t>
+        </is>
       </c>
       <c r="D60">
         <v>28890.9</v>
@@ -1317,14 +1374,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2">
-        <v>47483</v>
-      </c>
-      <c r="B61">
-        <v>262.5106168605735</v>
-      </c>
-      <c r="C61">
-        <v>204.2078068496785</v>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2029-12-31</t>
+        </is>
       </c>
       <c r="D61">
         <v>30008.6</v>
@@ -1334,14 +1387,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2">
-        <v>47848</v>
-      </c>
-      <c r="B62">
-        <v>262.5689812980181</v>
-      </c>
-      <c r="C62">
-        <v>204.242577755574</v>
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2030-12-31</t>
+        </is>
       </c>
       <c r="D62">
         <v>31160.4</v>

</xml_diff>

<commit_message>
Revert "Ad hoc fix to pull_data"
This reverts commit f045296798e0f6cb47160b354b82642fca7805f1.
</commit_message>
<xml_diff>
--- a/data/raw/haver/economic_annual.xlsx
+++ b/data/raw/haver/economic_annual.xlsx
@@ -15,6 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -52,11 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,6 +360,9 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
@@ -385,10 +392,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1970-12-31</t>
-        </is>
+      <c r="A2" s="2">
+        <v>25933</v>
       </c>
       <c r="D2">
         <v>1088</v>
@@ -398,10 +403,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1971-12-31</t>
-        </is>
+      <c r="A3" s="2">
+        <v>26298</v>
       </c>
       <c r="D3">
         <v>1177.4</v>
@@ -411,10 +414,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1972-12-31</t>
-        </is>
+      <c r="A4" s="2">
+        <v>26664</v>
       </c>
       <c r="D4">
         <v>1265.7</v>
@@ -424,10 +425,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1973-12-31</t>
-        </is>
+      <c r="A5" s="2">
+        <v>27029</v>
       </c>
       <c r="D5">
         <v>1378.8</v>
@@ -437,10 +436,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1974-12-31</t>
-        </is>
+      <c r="A6" s="2">
+        <v>27394</v>
       </c>
       <c r="D6">
         <v>1556</v>
@@ -450,10 +447,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1975-12-31</t>
-        </is>
+      <c r="A7" s="2">
+        <v>27759</v>
       </c>
       <c r="C7">
         <v>25.68916666666667</v>
@@ -466,10 +461,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1976-12-31</t>
-        </is>
+      <c r="A8" s="2">
+        <v>28125</v>
       </c>
       <c r="C8">
         <v>27.615</v>
@@ -482,10 +475,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1977-12-31</t>
-        </is>
+      <c r="A9" s="2">
+        <v>28490</v>
       </c>
       <c r="C9">
         <v>30.92</v>
@@ -498,10 +489,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1978-12-31</t>
-        </is>
+      <c r="A10" s="2">
+        <v>28855</v>
       </c>
       <c r="C10">
         <v>35.61166666666667</v>
@@ -514,10 +503,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1979-12-31</t>
-        </is>
+      <c r="A11" s="2">
+        <v>29220</v>
       </c>
       <c r="C11">
         <v>41.09416666666667</v>
@@ -530,10 +517,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1980-12-31</t>
-        </is>
+      <c r="A12" s="2">
+        <v>29586</v>
       </c>
       <c r="C12">
         <v>45.0925</v>
@@ -546,10 +531,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1981-12-31</t>
-        </is>
+      <c r="A13" s="2">
+        <v>29951</v>
       </c>
       <c r="C13">
         <v>47.96</v>
@@ -562,10 +545,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1982-12-31</t>
-        </is>
+      <c r="A14" s="2">
+        <v>30316</v>
       </c>
       <c r="C14">
         <v>48.94166666666666</v>
@@ -578,10 +559,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1983-12-31</t>
-        </is>
+      <c r="A15" s="2">
+        <v>30681</v>
       </c>
       <c r="C15">
         <v>50.45916666666667</v>
@@ -594,10 +573,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1984-12-31</t>
-        </is>
+      <c r="A16" s="2">
+        <v>31047</v>
       </c>
       <c r="C16">
         <v>52.84</v>
@@ -610,10 +587,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>1985-12-31</t>
-        </is>
+      <c r="A17" s="2">
+        <v>31412</v>
       </c>
       <c r="C17">
         <v>55.88500000000001</v>
@@ -626,10 +601,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1986-12-31</t>
-        </is>
+      <c r="A18" s="2">
+        <v>31777</v>
       </c>
       <c r="C18">
         <v>60.82166666666666</v>
@@ -642,10 +615,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1987-12-31</t>
-        </is>
+      <c r="A19" s="2">
+        <v>32142</v>
       </c>
       <c r="C19">
         <v>66.26833333333333</v>
@@ -658,10 +629,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>1988-12-31</t>
-        </is>
+      <c r="A20" s="2">
+        <v>32508</v>
       </c>
       <c r="C20">
         <v>71.14416666666666</v>
@@ -674,10 +643,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>1989-12-31</t>
-        </is>
+      <c r="A21" s="2">
+        <v>32873</v>
       </c>
       <c r="C21">
         <v>75.50833333333334</v>
@@ -690,10 +657,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>1990-12-31</t>
-        </is>
+      <c r="A22" s="2">
+        <v>33238</v>
       </c>
       <c r="C22">
         <v>76.935</v>
@@ -706,10 +671,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>1991-12-31</t>
-        </is>
+      <c r="A23" s="2">
+        <v>33603</v>
       </c>
       <c r="B23">
         <v>100.3075</v>
@@ -725,10 +688,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>1992-12-31</t>
-        </is>
+      <c r="A24" s="2">
+        <v>33969</v>
       </c>
       <c r="B24">
         <v>102.8225</v>
@@ -744,10 +705,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>1993-12-31</t>
-        </is>
+      <c r="A25" s="2">
+        <v>34334</v>
       </c>
       <c r="B25">
         <v>105.305</v>
@@ -763,10 +722,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>1994-12-31</t>
-        </is>
+      <c r="A26" s="2">
+        <v>34699</v>
       </c>
       <c r="B26">
         <v>108.82</v>
@@ -782,10 +739,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>1995-12-31</t>
-        </is>
+      <c r="A27" s="2">
+        <v>35064</v>
       </c>
       <c r="B27">
         <v>111.66</v>
@@ -801,10 +756,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>1996-12-31</t>
-        </is>
+      <c r="A28" s="2">
+        <v>35430</v>
       </c>
       <c r="B28">
         <v>114.94</v>
@@ -820,10 +773,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>1997-12-31</t>
-        </is>
+      <c r="A29" s="2">
+        <v>35795</v>
       </c>
       <c r="B29">
         <v>118.2175</v>
@@ -839,10 +790,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>1998-12-31</t>
-        </is>
+      <c r="A30" s="2">
+        <v>36160</v>
       </c>
       <c r="B30">
         <v>123.935</v>
@@ -858,10 +807,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>1999-12-31</t>
-        </is>
+      <c r="A31" s="2">
+        <v>36525</v>
       </c>
       <c r="B31">
         <v>131.4875</v>
@@ -877,10 +824,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2000-12-31</t>
-        </is>
+      <c r="A32" s="2">
+        <v>36891</v>
       </c>
       <c r="B32">
         <v>140.3075</v>
@@ -896,10 +841,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2001-12-31</t>
-        </is>
+      <c r="A33" s="2">
+        <v>37256</v>
       </c>
       <c r="B33">
         <v>150.0075</v>
@@ -915,10 +858,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2002-12-31</t>
-        </is>
+      <c r="A34" s="2">
+        <v>37621</v>
       </c>
       <c r="B34">
         <v>160.5775</v>
@@ -934,10 +875,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2003-12-31</t>
-        </is>
+      <c r="A35" s="2">
+        <v>37986</v>
       </c>
       <c r="B35">
         <v>172.8875</v>
@@ -953,10 +892,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2004-12-31</t>
-        </is>
+      <c r="A36" s="2">
+        <v>38352</v>
       </c>
       <c r="B36">
         <v>189.2175</v>
@@ -972,10 +909,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2005-12-31</t>
-        </is>
+      <c r="A37" s="2">
+        <v>38717</v>
       </c>
       <c r="B37">
         <v>209.0325</v>
@@ -991,10 +926,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2006-12-31</t>
-        </is>
+      <c r="A38" s="2">
+        <v>39082</v>
       </c>
       <c r="B38">
         <v>221.2775</v>
@@ -1010,10 +943,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2007-12-31</t>
-        </is>
+      <c r="A39" s="2">
+        <v>39447</v>
       </c>
       <c r="B39">
         <v>221.255</v>
@@ -1029,10 +960,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2008-12-31</t>
-        </is>
+      <c r="A40" s="2">
+        <v>39813</v>
       </c>
       <c r="B40">
         <v>203.2025</v>
@@ -1048,10 +977,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2009-12-31</t>
-        </is>
+      <c r="A41" s="2">
+        <v>40178</v>
       </c>
       <c r="B41">
         <v>191.0975</v>
@@ -1067,10 +994,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2010-12-31</t>
-        </is>
+      <c r="A42" s="2">
+        <v>40543</v>
       </c>
       <c r="B42">
         <v>185.3925</v>
@@ -1086,10 +1011,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>2011-12-31</t>
-        </is>
+      <c r="A43" s="2">
+        <v>40908</v>
       </c>
       <c r="B43">
         <v>177.56</v>
@@ -1105,10 +1028,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2012-12-31</t>
-        </is>
+      <c r="A44" s="2">
+        <v>41274</v>
       </c>
       <c r="B44">
         <v>182.57</v>
@@ -1124,10 +1045,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2013-12-31</t>
-        </is>
+      <c r="A45" s="2">
+        <v>41639</v>
       </c>
       <c r="B45">
         <v>195.37</v>
@@ -1143,10 +1062,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>2014-12-31</t>
-        </is>
+      <c r="A46" s="2">
+        <v>42004</v>
       </c>
       <c r="B46">
         <v>205.12</v>
@@ -1162,10 +1079,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>2015-12-31</t>
-        </is>
+      <c r="A47" s="2">
+        <v>42369</v>
       </c>
       <c r="B47">
         <v>215.915</v>
@@ -1181,10 +1096,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>2016-12-31</t>
-        </is>
+      <c r="A48" s="2">
+        <v>42735</v>
       </c>
       <c r="B48">
         <v>228.37</v>
@@ -1200,10 +1113,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>2017-12-31</t>
-        </is>
+      <c r="A49" s="2">
+        <v>43100</v>
       </c>
       <c r="B49">
         <v>242.775</v>
@@ -1219,10 +1130,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>2018-12-31</t>
-        </is>
+      <c r="A50" s="2">
+        <v>43465</v>
       </c>
       <c r="B50">
         <v>258.37</v>
@@ -1238,10 +1147,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>2019-12-31</t>
-        </is>
+      <c r="A51" s="2">
+        <v>43830</v>
       </c>
       <c r="B51">
         <v>271.9300000000001</v>
@@ -1257,10 +1164,14 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>2020-12-31</t>
-        </is>
+      <c r="A52" s="2">
+        <v>44196</v>
+      </c>
+      <c r="B52">
+        <v>257.6916666666667</v>
+      </c>
+      <c r="C52">
+        <v>201.2072222222222</v>
       </c>
       <c r="D52">
         <v>21763.5</v>
@@ -1270,10 +1181,14 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>2021-12-31</t>
-        </is>
+      <c r="A53" s="2">
+        <v>44561</v>
+      </c>
+      <c r="B53">
+        <v>262.6638888888889</v>
+      </c>
+      <c r="C53">
+        <v>204.4562962962963</v>
       </c>
       <c r="D53">
         <v>22257.4</v>
@@ -1283,10 +1198,14 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>2022-12-31</t>
-        </is>
+      <c r="A54" s="2">
+        <v>44926</v>
+      </c>
+      <c r="B54">
+        <v>264.0951851851852</v>
+      </c>
+      <c r="C54">
+        <v>205.0889506172839</v>
       </c>
       <c r="D54">
         <v>23013.9</v>
@@ -1296,10 +1215,14 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>2023-12-31</t>
-        </is>
+      <c r="A55" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B55">
+        <v>261.4835802469136</v>
+      </c>
+      <c r="C55">
+        <v>203.5841563786008</v>
       </c>
       <c r="D55">
         <v>23874.9</v>
@@ -1309,10 +1232,14 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>2024-12-31</t>
-        </is>
+      <c r="A56" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B56">
+        <v>262.7475514403292</v>
+      </c>
+      <c r="C56">
+        <v>204.3764677640603</v>
       </c>
       <c r="D56">
         <v>24806.6</v>
@@ -1322,10 +1249,14 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>2025-12-31</t>
-        </is>
+      <c r="A57" s="2">
+        <v>46022</v>
+      </c>
+      <c r="B57">
+        <v>262.775438957476</v>
+      </c>
+      <c r="C57">
+        <v>204.349858253315</v>
       </c>
       <c r="D57">
         <v>25781</v>
@@ -1335,10 +1266,14 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>2026-12-31</t>
-        </is>
+      <c r="A58" s="2">
+        <v>46387</v>
+      </c>
+      <c r="B58">
+        <v>262.3355235482396</v>
+      </c>
+      <c r="C58">
+        <v>204.1034941319921</v>
       </c>
       <c r="D58">
         <v>26784.5</v>
@@ -1348,10 +1283,14 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>2027-12-31</t>
-        </is>
+      <c r="A59" s="2">
+        <v>46752</v>
+      </c>
+      <c r="B59">
+        <v>262.6195046486816</v>
+      </c>
+      <c r="C59">
+        <v>204.2766067164558</v>
       </c>
       <c r="D59">
         <v>27817.3</v>
@@ -1361,10 +1300,14 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>2028-12-31</t>
-        </is>
+      <c r="A60" s="2">
+        <v>47118</v>
+      </c>
+      <c r="B60">
+        <v>262.5768223847991</v>
+      </c>
+      <c r="C60">
+        <v>204.2433197005876</v>
       </c>
       <c r="D60">
         <v>28890.9</v>
@@ -1374,10 +1317,14 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>2029-12-31</t>
-        </is>
+      <c r="A61" s="2">
+        <v>47483</v>
+      </c>
+      <c r="B61">
+        <v>262.5106168605735</v>
+      </c>
+      <c r="C61">
+        <v>204.2078068496785</v>
       </c>
       <c r="D61">
         <v>30008.6</v>
@@ -1387,10 +1334,14 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>2030-12-31</t>
-        </is>
+      <c r="A62" s="2">
+        <v>47848</v>
+      </c>
+      <c r="B62">
+        <v>262.5689812980181</v>
+      </c>
+      <c r="C62">
+        <v>204.242577755574</v>
       </c>
       <c r="D62">
         <v>31160.4</v>

</xml_diff>